<commit_message>
atualização do módulo para inclusão das funções de registro de andamento e atualização de histórico
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m913685\Documents\Uadson\repos\automacao-processo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591E5559-30CF-4D9B-9506-CE32E2370286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2334E8-3DA0-4806-96B9-83EEE980A2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="1350" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="obj" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -361,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.42578125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -374,27 +374,52 @@
   <sheetData>
     <row r="1" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
-        <v>87321444</v>
+        <v>87369811</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>87321185</v>
+        <v>87369552</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>87321118</v>
+        <v>87369391</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>87320529</v>
+        <v>87369170</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>87320201</v>
+        <v>87369030</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>87368891</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>87368629</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>87145832</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>87162117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>87364267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
insercao de datas automaticas
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m913685\Documents\Uadson\repos\automacao-processo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2334E8-3DA0-4806-96B9-83EEE980A2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599CD343-F536-4314-9A22-A252C585B08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="1350" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.42578125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -374,52 +374,107 @@
   <sheetData>
     <row r="1" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
-        <v>87369811</v>
+        <v>87161749</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>87369552</v>
+        <v>87369811</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>87369391</v>
+        <v>87369552</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>87369170</v>
+        <v>87369391</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>87369030</v>
+        <v>87369170</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>87368891</v>
+        <v>87369030</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>87368629</v>
+        <v>87368891</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>87145832</v>
+        <v>87368629</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>87162117</v>
+        <v>87145832</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
+        <v>87162117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>87364267</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>87145620</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>87145506</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>87145280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>87145131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>87144950</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>87144682</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>87144445</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>87162397</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>87162214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>87162559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>